<commit_message>
retry (failing because os opened excel file) RP before module state preservation..
</commit_message>
<xml_diff>
--- a/docs/FilteringTemplate.xlsx
+++ b/docs/FilteringTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="24840" windowHeight="10845"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="24840" windowHeight="10845"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,6 +105,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,7 +139,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +428,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.28515625" customWidth="1"/>
   </cols>
@@ -466,118 +470,123 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>456</v>
+        <v>264</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1">
-        <v>44090</v>
+        <v>43861</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>78</v>
+        <v>253</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>44065</v>
+        <v>43878</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>902</v>
+        <v>664</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
-        <v>44157</v>
+        <v>43897</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1232</v>
+        <v>543</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
-        <v>43959</v>
+        <v>43930</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>543</v>
+        <v>1232</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>43930</v>
+        <v>43593</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>664</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
-        <v>43897</v>
+        <v>43699</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>253</v>
+        <v>456</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>43878</v>
+        <v>43724</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>264</v>
+        <v>902</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>43861</v>
+        <v>43791</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F10"/>
+  <autoFilter ref="A1:F10">
+    <sortState ref="A2:F10">
+      <sortCondition ref="C1:C10"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>